<commit_message>
[documentation] latex file added
</commit_message>
<xml_diff>
--- a/documentation/usecase diagram/realization/usecase realization.xlsx
+++ b/documentation/usecase diagram/realization/usecase realization.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="62">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -92,6 +92,12 @@
   </si>
   <si>
     <t xml:space="preserve">اعلام کردن حادثه</t>
+  </si>
+  <si>
+    <t xml:space="preserve">بعدا تو نمودار کلاس چک بشه که با  راننده ارتباط داشته باشه</t>
+  </si>
+  <si>
+    <t xml:space="preserve">مدیر احراز هویت، راننده</t>
   </si>
   <si>
     <t xml:space="preserve">تایید کردن اطلاعات راننده و تحصیص شناسه کاربری و رمز عبور</t>
@@ -214,6 +220,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -235,19 +242,39 @@
       <sz val="10"/>
       <name val="Lohit Devanagari"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Lohit Devanagari"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFBF00"/>
+        <bgColor rgb="FFFF9900"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFA6A6"/>
+        <bgColor rgb="FFFFCC99"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -284,7 +311,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -293,7 +320,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -306,6 +345,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFFA6A6"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFBF00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -316,11 +415,11 @@
   </sheetPr>
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="40.75"/>
@@ -349,7 +448,7 @@
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="D3" s="3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -360,7 +459,7 @@
       <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" s="3" t="n">
         <v>2</v>
       </c>
     </row>
@@ -371,62 +470,62 @@
       <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="D5" s="3" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="2" t="n">
+      <c r="D6" s="3" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="2" t="n">
+      <c r="D7" s="3" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="2" t="n">
+      <c r="D8" s="3" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="2" t="n">
+      <c r="D9" s="3" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="2" t="n">
+      <c r="D10" s="3" t="n">
         <v>8</v>
       </c>
     </row>
@@ -437,29 +536,29 @@
       <c r="C11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="2" t="n">
+      <c r="D11" s="3" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="2" t="n">
+      <c r="D12" s="3" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="2" t="n">
+      <c r="D13" s="3" t="n">
         <v>11</v>
       </c>
     </row>
@@ -470,7 +569,7 @@
       <c r="C14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="2" t="n">
+      <c r="D14" s="3" t="n">
         <v>12</v>
       </c>
     </row>
@@ -481,260 +580,263 @@
       <c r="C15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="2" t="n">
+      <c r="D15" s="3" t="n">
         <v>13</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>24</v>
+      </c>
       <c r="B16" s="2" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="D16" s="3" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="2" t="n">
+      <c r="B17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="3" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="2" t="n">
+      <c r="B18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="3" t="n">
         <v>16</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="3" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="3" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="3" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="3" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="3" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="3" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="3" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" s="3" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="3" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="3" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D29" s="3" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="3" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D31" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="C19" s="2" t="s">
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D32" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="D19" s="2" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="2" t="s">
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D33" s="3" t="n">
         <v>31</v>
       </c>
-      <c r="C20" s="2" t="s">
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D34" s="3" t="n">
         <v>32</v>
       </c>
-      <c r="D20" s="2" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="2" t="s">
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D35" s="3" t="n">
         <v>33</v>
       </c>
-      <c r="C21" s="2" t="s">
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D36" s="3" t="n">
         <v>34</v>
       </c>
-      <c r="D21" s="2" t="n">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="2" t="s">
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D37" s="3" t="n">
         <v>35</v>
       </c>
-      <c r="D22" s="2" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D23" s="2" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" s="2" t="n">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D25" s="2" t="n">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D26" s="2" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D27" s="2" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D28" s="2" t="n">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D29" s="2" t="n">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D30" s="2" t="n">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D31" s="2" t="n">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D32" s="2" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D33" s="2" t="n">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D34" s="2" t="n">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D35" s="2" t="n">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D36" s="2" t="n">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D37" s="2" t="n">
-        <v>35</v>
-      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D38" s="2" t="n">
+      <c r="B38" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D38" s="3" t="n">
         <v>36</v>
       </c>
     </row>

</xml_diff>